<commit_message>
criado os graficos qtde_veiculos, qtde_veiculos_carga, qtde_pessoas e corrigido as notas de rodapé das imagens e figuras.
</commit_message>
<xml_diff>
--- a/data-raw/quantidade_pessoas.xlsx
+++ b/data-raw/quantidade_pessoas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="21">
   <si>
     <t xml:space="preserve">mês</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018</t>
   </si>
 </sst>
 </file>
@@ -185,13 +188,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D56" activeCellId="0" sqref="D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.52"/>
   </cols>
@@ -796,6 +799,174 @@
       </c>
       <c r="D43" s="0" t="n">
         <v>426</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>952</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>478</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>521</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>743</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>653</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>461</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>940</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>576</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>530</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>553</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>605</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>1082</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>1127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>